<commit_message>
added highlight to outlier CT values
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamboudy/Desktop/research/qPCR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamboudy/Desktop/programs/qpcr-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60F7CDFB-32C1-1A49-A344-727E0C003C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123B816D-59D4-0445-9B57-DCF3F5501680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="1740" windowWidth="17180" windowHeight="11240" xr2:uid="{0B55963A-F6EE-4E40-ADE3-FA50BA9E8000}"/>
+    <workbookView xWindow="8180" yWindow="2060" windowWidth="19740" windowHeight="14660" activeTab="2" xr2:uid="{0B55963A-F6EE-4E40-ADE3-FA50BA9E8000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw data" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="sample loading table tab" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1220,7 +1219,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.9737537701924639</c:v>
+                  <c:v>6.9737537701924603</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>9.6227045059204102</c:v>
@@ -3465,7 +3464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8CC3CC-9DE4-1B4E-9100-EF58579FE3AA}">
   <dimension ref="A1:AL140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="I117" sqref="I117:I132"/>
     </sheetView>
   </sheetViews>
@@ -15066,7 +15065,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15227,8 +15226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3C8B4F-E563-7B4B-AC1F-4ACADF87B813}">
   <dimension ref="A1:W136"/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="O58" sqref="O58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -15285,26 +15284,26 @@
       </c>
       <c r="E2">
         <f>(C2-$O$59)/$O$58</f>
-        <v>9.0755927810352226</v>
+        <v>9.0755927810352208</v>
       </c>
       <c r="F2" s="3">
         <f>10^E2</f>
-        <v>1190125555.9384029</v>
+        <v>1190125555.9383943</v>
       </c>
       <c r="G2" s="3">
         <f>F2*4520*2</f>
-        <v>10758735025683.162</v>
+        <v>10758735025683.084</v>
       </c>
       <c r="H2" t="s">
         <v>270</v>
       </c>
       <c r="I2" s="3">
         <f>AVERAGE(G2:G4)</f>
-        <v>10270369963584.617</v>
+        <v>10270369963584.557</v>
       </c>
       <c r="J2">
         <f>STDEV(G2:G4)</f>
-        <v>919564348925.53455</v>
+        <v>919564348925.54004</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -15316,15 +15315,15 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E31" si="0">(C3-$O$59)/$O$58</f>
-        <v>9.0080749872776877</v>
+        <v>9.0080749872776842</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F31" si="1">10^E3</f>
-        <v>1018767277.9007785</v>
+        <v>1018767277.9007713</v>
       </c>
       <c r="G3" s="3">
         <f t="shared" ref="G3:G31" si="2">F3*4520*2</f>
-        <v>9209656192223.0371</v>
+        <v>9209656192222.9727</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -15336,15 +15335,15 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>9.0789697591606</v>
+        <v>9.0789697591605982</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="1"/>
-        <v>1199415782.3946519</v>
+        <v>1199415782.3946478</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" si="2"/>
-        <v>10842718672847.652</v>
+        <v>10842718672847.617</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -15363,26 +15362,26 @@
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>0.74931116135594866</v>
+        <v>0.74931116135594988</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
-        <v>5.6145009719924719</v>
+        <v>5.6145009719924861</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" si="2"/>
-        <v>50755.088786811946</v>
+        <v>50755.088786812077</v>
       </c>
       <c r="H5" t="s">
         <v>271</v>
       </c>
       <c r="I5" s="3">
         <f>AVERAGE(G5:G7)</f>
-        <v>50440.197838223794</v>
+        <v>50440.197838223925</v>
       </c>
       <c r="J5">
         <f>STDEV(G5:G7)</f>
-        <v>1237.1400353035906</v>
+        <v>1237.1400353035999</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -15394,15 +15393,15 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0.73470110510431808</v>
+        <v>0.7347011051043193</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" si="1"/>
-        <v>5.428765784398907</v>
+        <v>5.4287657843989212</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" si="2"/>
-        <v>49076.042690966118</v>
+        <v>49076.042690966249</v>
       </c>
     </row>
     <row r="7" spans="1:23">
@@ -15414,15 +15413,15 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0.75554992385664499</v>
+        <v>0.75554992385664621</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="1"/>
-        <v>5.6957369509837736</v>
+        <v>5.6957369509837905</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="2"/>
-        <v>51489.46203689331</v>
+        <v>51489.462036893463</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -15441,26 +15440,26 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>5.0270333993333738</v>
+        <v>5.0270333993333729</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="1"/>
-        <v>106422.48590848441</v>
+        <v>106422.48590848403</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="2"/>
-        <v>962059272.61269903</v>
+        <v>962059272.61269557</v>
       </c>
       <c r="H8" t="s">
         <v>272</v>
       </c>
       <c r="I8" s="3">
         <f>AVERAGE(G8:G10)</f>
-        <v>928907534.686257</v>
+        <v>928907534.68625486</v>
       </c>
       <c r="J8">
         <f>STDEV(G8:G10)</f>
-        <v>48104677.711788855</v>
+        <v>48104677.711788177</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -15472,15 +15471,15 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>5.02197982433281</v>
+        <v>5.0219798243328091</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="1"/>
-        <v>105191.30048171432</v>
+        <v>105191.30048171413</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="2"/>
-        <v>950929356.35469747</v>
+        <v>950929356.3546958</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -15492,15 +15491,15 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>4.9852107930787062</v>
+        <v>4.9852107930787053</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="1"/>
-        <v>96651.988395063541</v>
+        <v>96651.988395063367</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="2"/>
-        <v>873733975.0913744</v>
+        <v>873733975.09137285</v>
       </c>
       <c r="P10" t="s">
         <v>98</v>
@@ -15543,22 +15542,22 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>3.4143011991533809</v>
+        <v>3.4143011991533814</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="1"/>
-        <v>2595.9791446979721</v>
+        <v>2595.9791446979743</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="2"/>
-        <v>23467651.468069669</v>
+        <v>23467651.468069687</v>
       </c>
       <c r="H11" t="s">
         <v>273</v>
       </c>
       <c r="I11" s="3">
         <f>AVERAGE(G12:G13)</f>
-        <v>21897049.100618877</v>
+        <v>21897049.100618899</v>
       </c>
       <c r="J11">
         <f>STDEV(G11:G13)</f>
@@ -15598,15 +15597,15 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>3.4095814116528542</v>
+        <v>3.4095814116528547</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="1"/>
-        <v>2567.919538146366</v>
+        <v>2567.9195381463683</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="2"/>
-        <v>23213992.62484315</v>
+        <v>23213992.624843169</v>
       </c>
       <c r="P12" t="s">
         <v>108</v>
@@ -15642,15 +15641,15 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>3.3572791678970169</v>
+        <v>3.3572791678970173</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="1"/>
-        <v>2276.5603513710848</v>
+        <v>2276.5603513710867</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="2"/>
-        <v>20580105.576394606</v>
+        <v>20580105.576394625</v>
       </c>
       <c r="P13" t="s">
         <v>109</v>
@@ -15693,26 +15692,26 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>8.1261209340542546</v>
+        <v>8.1261209340542528</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>133696775.80294503</v>
+        <v>133696775.80294456</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="2"/>
-        <v>1208618853258.623</v>
+        <v>1208618853258.6189</v>
       </c>
       <c r="H14" t="s">
         <v>274</v>
       </c>
       <c r="I14" s="3">
         <f>AVERAGE(G14:G16)</f>
-        <v>1425449909704.043</v>
+        <v>1425449909704.0378</v>
       </c>
       <c r="J14">
         <f>STDEV(G14:G16)</f>
-        <v>216084795630.44016</v>
+        <v>216084795630.44141</v>
       </c>
       <c r="P14" t="s">
         <v>110</v>
@@ -15748,15 +15747,15 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>8.2588820903190712</v>
+        <v>8.2588820903190694</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>181502282.24889484</v>
+        <v>181502282.24889418</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="2"/>
-        <v>1640780631530.0093</v>
+        <v>1640780631530.0034</v>
       </c>
       <c r="P15" t="s">
         <v>111</v>
@@ -15792,15 +15791,15 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>8.1982403996873039</v>
+        <v>8.1982403996873021</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="1"/>
-        <v>157848478.35436907</v>
+        <v>157848478.35436851</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="2"/>
-        <v>1426950244323.4963</v>
+        <v>1426950244323.4912</v>
       </c>
       <c r="P16" t="s">
         <v>118</v>
@@ -15843,26 +15842,26 @@
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>4.8647739743152645</v>
+        <v>4.8647739743152636</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="1"/>
-        <v>73244.323869725893</v>
+        <v>73244.323869725762</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="2"/>
-        <v>662128687.78232205</v>
+        <v>662128687.78232086</v>
       </c>
       <c r="H17" t="s">
         <v>252</v>
       </c>
       <c r="I17" s="3">
         <f>AVERAGE(G17:G19)</f>
-        <v>611856923.91199553</v>
+        <v>611856923.91199505</v>
       </c>
       <c r="J17">
         <f>STDEV(G17:G19)</f>
-        <v>50570616.661268577</v>
+        <v>50570616.661267981</v>
       </c>
       <c r="P17" t="s">
         <v>119</v>
@@ -16008,11 +16007,11 @@
       </c>
       <c r="I20" s="3">
         <f>AVERAGE(G20:G22)</f>
-        <v>2137821572.5261314</v>
+        <v>2137821572.5261304</v>
       </c>
       <c r="J20">
         <f>STDEV(G20:G22)</f>
-        <v>418199427.06727231</v>
+        <v>418199427.06727475</v>
       </c>
       <c r="P20" t="s">
         <v>122</v>
@@ -16092,15 +16091,15 @@
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>5.2633130243597446</v>
+        <v>5.2633130243597437</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="1"/>
-        <v>183363.55669475321</v>
+        <v>183363.55669475289</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="2"/>
-        <v>1657606552.5205691</v>
+        <v>1657606552.520566</v>
       </c>
       <c r="P22" t="s">
         <v>130</v>
@@ -16293,26 +16292,26 @@
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>7.2314748933294055</v>
+        <v>7.2314748933294046</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="1"/>
-        <v>17040208.066069733</v>
+        <v>17040208.066069674</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" si="2"/>
-        <v>154043480917.27039</v>
+        <v>154043480917.26984</v>
       </c>
       <c r="H26" t="s">
         <v>277</v>
       </c>
       <c r="I26" s="3">
         <f>AVERAGE(G26:G28)</f>
-        <v>88679278632.248886</v>
+        <v>88679278632.248642</v>
       </c>
       <c r="J26">
         <f>STDEV(G26:G28)</f>
-        <v>56618447036.234886</v>
+        <v>56618447036.23465</v>
       </c>
       <c r="P26" t="s">
         <v>134</v>
@@ -16348,15 +16347,15 @@
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
-        <v>6.7831007245293637</v>
+        <v>6.7831007245293629</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="1"/>
-        <v>6068770.6432320448</v>
+        <v>6068770.6432320336</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="2"/>
-        <v>54861686614.817688</v>
+        <v>54861686614.817581</v>
       </c>
       <c r="P27" t="s">
         <v>135</v>
@@ -16392,15 +16391,15 @@
       </c>
       <c r="E28">
         <f t="shared" si="0"/>
-        <v>6.8007160776563298</v>
+        <v>6.8007160776563289</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="1"/>
-        <v>6319985.43856843</v>
+        <v>6319985.4385684188</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" si="2"/>
-        <v>57132668364.658607</v>
+        <v>57132668364.658508</v>
       </c>
       <c r="P28" t="s">
         <v>142</v>
@@ -16443,26 +16442,26 @@
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
-        <v>4.884542418067471</v>
+        <v>4.8845424180674701</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>76655.340670501377</v>
+        <v>76655.340670501231</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="2"/>
-        <v>692964279.66133249</v>
+        <v>692964279.66133118</v>
       </c>
       <c r="H29" t="s">
         <v>278</v>
       </c>
       <c r="I29" s="3">
         <f>AVERAGE(G29:G31)</f>
-        <v>690281938.14445639</v>
+        <v>690281938.14445543</v>
       </c>
       <c r="J29">
         <f>STDEV(G29:G31)</f>
-        <v>12192210.63691714</v>
+        <v>12192210.636916477</v>
       </c>
       <c r="P29" t="s">
         <v>143</v>
@@ -16498,15 +16497,15 @@
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
-        <v>4.8894935993180235</v>
+        <v>4.8894935993180226</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="1"/>
-        <v>77534.251618829701</v>
+        <v>77534.25161882957</v>
       </c>
       <c r="G30" s="3">
         <f t="shared" si="2"/>
-        <v>700909634.63422048</v>
+        <v>700909634.63421929</v>
       </c>
       <c r="P30" t="s">
         <v>144</v>
@@ -17135,7 +17134,7 @@
       </c>
       <c r="O58">
         <f>SLOPE(L59:L66,K59:K66)</f>
-        <v>-2.3657037303561252</v>
+        <v>-2.3657037303561261</v>
       </c>
     </row>
     <row r="59" spans="1:15">
@@ -17154,14 +17153,14 @@
         <v>10</v>
       </c>
       <c r="L59">
-        <v>6.9737537701924639</v>
+        <v>6.9737537701924603</v>
       </c>
       <c r="N59" s="3" t="s">
         <v>281</v>
       </c>
       <c r="O59">
         <f>INTERCEPT(L59:L66,K59:K66)</f>
-        <v>30.761625641868225</v>
+        <v>30.761625641868228</v>
       </c>
     </row>
     <row r="60" spans="1:15">

</xml_diff>

<commit_message>
fixed errors in removing values from CT list, there is a bug with how stds are extrapolated in plot function
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamboudy/Desktop/programs/qpcr-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123B816D-59D4-0445-9B57-DCF3F5501680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59FF406-CBE9-8F40-9B6B-1C2CBB21FE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="2060" windowWidth="19740" windowHeight="14660" activeTab="2" xr2:uid="{0B55963A-F6EE-4E40-ADE3-FA50BA9E8000}"/>
+    <workbookView xWindow="8180" yWindow="1760" windowWidth="19740" windowHeight="14660" xr2:uid="{0B55963A-F6EE-4E40-ADE3-FA50BA9E8000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw data" sheetId="2" r:id="rId1"/>
@@ -3464,8 +3464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8CC3CC-9DE4-1B4E-9100-EF58579FE3AA}">
   <dimension ref="A1:AL140"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I117" sqref="I117:I132"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -4407,7 +4407,7 @@
         <v>103</v>
       </c>
       <c r="I49" s="2">
-        <v>29.023540496826172</v>
+        <v>30</v>
       </c>
       <c r="J49" s="2">
         <v>21.004676818847656</v>
@@ -15226,8 +15226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3C8B4F-E563-7B4B-AC1F-4ACADF87B813}">
   <dimension ref="A1:W136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="O58" sqref="O58"/>
+    <sheetView zoomScale="106" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -15358,7 +15358,7 @@
       </c>
       <c r="D5">
         <f>AVERAGE(C5:C7)</f>
-        <v>28.995578765869141</v>
+        <v>29.321065266927082</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -15377,11 +15377,11 @@
       </c>
       <c r="I5" s="3">
         <f>AVERAGE(G5:G7)</f>
-        <v>50440.197838223925</v>
+        <v>40405.516315871791</v>
       </c>
       <c r="J5">
         <f>STDEV(G5:G7)</f>
-        <v>1237.1400353035999</v>
+        <v>18565.60267218604</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -15389,19 +15389,19 @@
         <v>110</v>
       </c>
       <c r="C6" s="9">
-        <v>29.023540496826172</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0.7347011051043193</v>
+        <v>0.32194464255825284</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" si="1"/>
-        <v>5.4287657843989212</v>
+        <v>2.0986723588395844</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" si="2"/>
-        <v>49076.042690966249</v>
+        <v>18971.998123909842</v>
       </c>
     </row>
     <row r="7" spans="1:23">

</xml_diff>